<commit_message>
done for the day. aug 17. implemented dropdown menus and objects
</commit_message>
<xml_diff>
--- a/django_proj/data/Letter Tracking fields (1).xlsx
+++ b/django_proj/data/Letter Tracking fields (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\OneDrive\Documents\wsl\git\Letter_tracking\django_proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F725AE0-3129-4BC4-890D-1EE73A4EAA29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA07560-BD4D-48A4-99CF-1C2377953CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C82B721F-DD68-4537-A84B-D6CA80EA00D5}"/>
   </bookViews>
@@ -3167,12 +3167,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3187,7 +3193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3201,6 +3207,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3519,8 +3531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F841C79-5F93-4BFE-8EAC-4F26F9AED322}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3552,19 +3564,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="150.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>1010</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>198</v>
       </c>
     </row>
@@ -3594,55 +3606,56 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3735,36 +3748,36 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="7" t="s">
         <v>1009</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="7" t="s">
         <v>1009</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3822,41 +3835,43 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="7" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="7" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="7" t="s">
         <v>1007</v>
       </c>
     </row>
@@ -3967,7 +3982,7 @@
   <dimension ref="A1:M541"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Safety submit, tues aug 18. All code running, most attributes set to embassy standard
</commit_message>
<xml_diff>
--- a/django_proj/data/Letter Tracking fields (1).xlsx
+++ b/django_proj/data/Letter Tracking fields (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\OneDrive\Documents\wsl\git\Letter_tracking\django_proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA07560-BD4D-48A4-99CF-1C2377953CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC4DE64-C6CF-4D44-95D3-AB5D89A53CAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C82B721F-DD68-4537-A84B-D6CA80EA00D5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3445" uniqueCount="1022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="1023">
   <si>
     <t>Código</t>
   </si>
@@ -3144,6 +3144,9 @@
   </si>
   <si>
     <t>remove party affiliation</t>
+  </si>
+  <si>
+    <t>None Selected</t>
   </si>
 </sst>
 </file>
@@ -3167,7 +3170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3177,6 +3180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3193,7 +3202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3213,6 +3222,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3531,8 +3546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F841C79-5F93-4BFE-8EAC-4F26F9AED322}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3581,27 +3596,28 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3677,36 +3693,36 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="7" t="s">
         <v>1010</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="7" t="s">
         <v>1010</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="7" t="s">
         <v>111</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -3717,33 +3733,34 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="7" t="s">
         <v>1006</v>
       </c>
     </row>
@@ -3781,7 +3798,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>199</v>
       </c>
@@ -3799,7 +3816,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="232" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -3818,19 +3835,19 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="9" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3981,8 +3998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC6ECD6-7E08-4080-92D2-AA9150F9F03B}">
   <dimension ref="A1:M541"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4126,7 +4143,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -4138,6 +4155,9 @@
       </c>
       <c r="D6" s="3" t="s">
         <v>78</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>1022</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>196</v>

</xml_diff>

<commit_message>
thursday 20/8 progress, pushing before i restructure the models, which broke the app last time
</commit_message>
<xml_diff>
--- a/django_proj/data/Letter Tracking fields (1).xlsx
+++ b/django_proj/data/Letter Tracking fields (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\OneDrive\Documents\wsl\git\Letter_tracking\django_proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC4DE64-C6CF-4D44-95D3-AB5D89A53CAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB85658D-5E21-48CB-A55A-37108609C6D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C82B721F-DD68-4537-A84B-D6CA80EA00D5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="1023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3448" uniqueCount="1025">
   <si>
     <t>Código</t>
   </si>
@@ -3147,6 +3147,12 @@
   </si>
   <si>
     <t>None Selected</t>
+  </si>
+  <si>
+    <t>make two spaces- list?</t>
+  </si>
+  <si>
+    <t>multiple dropdown</t>
   </si>
 </sst>
 </file>
@@ -3547,7 +3553,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3814,7 +3820,9 @@
       <c r="E16" s="3" t="s">
         <v>1012</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
@@ -3832,7 +3840,9 @@
       <c r="E17" s="3" t="s">
         <v>1013</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>1024</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">

</xml_diff>

<commit_message>
slight changes, some migrations
</commit_message>
<xml_diff>
--- a/django_proj/data/Letter Tracking fields (1).xlsx
+++ b/django_proj/data/Letter Tracking fields (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\OneDrive\Documents\wsl\git\Letter_tracking\django_proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB85658D-5E21-48CB-A55A-37108609C6D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C502E7-A110-4B67-94DD-99DCCAAD1D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C82B721F-DD68-4537-A84B-D6CA80EA00D5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{C82B721F-DD68-4537-A84B-D6CA80EA00D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Info card w details" sheetId="2" r:id="rId1"/>
@@ -3146,13 +3146,13 @@
     <t>remove party affiliation</t>
   </si>
   <si>
-    <t>None Selected</t>
-  </si>
-  <si>
     <t>make two spaces- list?</t>
   </si>
   <si>
     <t>multiple dropdown</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -3176,7 +3176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3191,7 +3191,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3208,7 +3220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3235,6 +3247,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3552,8 +3573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F841C79-5F93-4BFE-8EAC-4F26F9AED322}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3739,17 +3760,17 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="9" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3805,59 +3826,59 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="11" t="s">
         <v>1012</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="11" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F17" s="13" t="s">
         <v>1023</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="6" t="s">
+    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
+      <c r="C18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="11" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4008,8 +4029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC6ECD6-7E08-4080-92D2-AA9150F9F03B}">
   <dimension ref="A1:M541"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4153,7 +4174,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -4167,7 +4188,7 @@
         <v>78</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>196</v>

</xml_diff>